<commit_message>
near complete top level schematic routing
</commit_message>
<xml_diff>
--- a/docs/XEM7310.xlsx
+++ b/docs/XEM7310.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koer2434/Google Drive/UST/research/covg/pcb_design/kicad/covg_daq_v2/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45517BA1-9FD0-FB4E-9BFB-A9B2C9133D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C1A353-7B8A-D743-9CC9-1E70A35D5896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440"/>
+    <workbookView minimized="1" xWindow="940" yWindow="-140" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XEM7310" sheetId="1" r:id="rId1"/>
@@ -1371,7 +1371,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2205,14 +2205,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>